<commit_message>
atualização do cronograma; pipeline de exemplo;
</commit_message>
<xml_diff>
--- a/docs/Cronograma_Grupo4.xlsx
+++ b/docs/Cronograma_Grupo4.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Facul\2022.1\Projeto e Contrucao de sistemas\Projeto\G1-P4-Airflow\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59AD576-9010-4745-B994-EDE0F0813340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="690" yWindow="2295" windowWidth="21600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Página1" sheetId="1" r:id="rId4"/>
+    <sheet name="Página1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t>status</t>
   </si>
@@ -40,39 +49,45 @@
     <t>Atrasado</t>
   </si>
   <si>
-    <t>Construção do pipeline</t>
-  </si>
-  <si>
     <t>Pronto</t>
+  </si>
+  <si>
+    <t>Construção do pipeline de exemplo</t>
+  </si>
+  <si>
+    <t>Início do pipeline do appraisal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -83,7 +98,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -117,7 +132,13 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -131,147 +152,129 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="18">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="4">
     <dxf>
-      <font/>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFB7E1CD"/>
           <bgColor rgb="FFB7E1CD"/>
         </patternFill>
       </fill>
-      <border/>
     </dxf>
     <dxf>
-      <font/>
       <fill>
-        <patternFill patternType="none"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE8F0FE"/>
+          <bgColor rgb="FFE8F0FE"/>
+        </patternFill>
       </fill>
-      <border/>
     </dxf>
     <dxf>
-      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF5B95F9"/>
           <bgColor rgb="FF5B95F9"/>
         </patternFill>
       </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE8F0FE"/>
-          <bgColor rgb="FFE8F0FE"/>
-        </patternFill>
-      </fill>
-      <border/>
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle count="3" pivot="0" name="Página1-style">
-      <tableStyleElement dxfId="2" type="headerRow"/>
-      <tableStyleElement dxfId="3" type="firstRowStripe"/>
-      <tableStyleElement dxfId="4" type="secondRowStripe"/>
+    <tableStyle name="Página1-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="headerRow" dxfId="3"/>
+      <tableStyleElement type="firstRowStripe" dxfId="2"/>
+      <tableStyleElement type="secondRowStripe" dxfId="1"/>
     </tableStyle>
   </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A1:W8" displayName="Table_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:W8" headerRowCount="0">
   <tableColumns count="23">
-    <tableColumn name="Column1" id="1"/>
-    <tableColumn name="Column2" id="2"/>
-    <tableColumn name="Column3" id="3"/>
-    <tableColumn name="Column4" id="4"/>
-    <tableColumn name="Column5" id="5"/>
-    <tableColumn name="Column6" id="6"/>
-    <tableColumn name="Column7" id="7"/>
-    <tableColumn name="Column8" id="8"/>
-    <tableColumn name="Column9" id="9"/>
-    <tableColumn name="Column10" id="10"/>
-    <tableColumn name="Column11" id="11"/>
-    <tableColumn name="Column12" id="12"/>
-    <tableColumn name="Column13" id="13"/>
-    <tableColumn name="Column14" id="14"/>
-    <tableColumn name="Column15" id="15"/>
-    <tableColumn name="Column16" id="16"/>
-    <tableColumn name="Column17" id="17"/>
-    <tableColumn name="Column18" id="18"/>
-    <tableColumn name="Column19" id="19"/>
-    <tableColumn name="Column20" id="20"/>
-    <tableColumn name="Column21" id="21"/>
-    <tableColumn name="Column22" id="22"/>
-    <tableColumn name="Column23" id="23"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Column3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Column4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Column5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Column6"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Column7"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Column8"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Column9"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Column10"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Column11"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Column12"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Column13"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Column14"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Column15"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Column16"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Column17"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Column18"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Column19"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Column20"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Column21"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Column22"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Column23"/>
   </tableColumns>
-  <tableStyleInfo name="Página1-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="Página1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
@@ -281,7 +284,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -471,32 +474,35 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:W10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="6.0" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection activeCell="H2" sqref="H2" pane="topRight"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="6" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="4.38"/>
-    <col customWidth="1" min="2" max="2" width="5.63"/>
-    <col customWidth="1" min="3" max="3" width="3.63"/>
-    <col customWidth="1" min="4" max="4" width="3.75"/>
-    <col customWidth="1" min="5" max="5" width="5.75"/>
-    <col customWidth="1" min="6" max="6" width="41.13"/>
-    <col customWidth="1" min="7" max="23" width="5.63"/>
+    <col min="1" max="1" width="4.42578125" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" customWidth="1"/>
+    <col min="3" max="3" width="3.5703125" customWidth="1"/>
+    <col min="4" max="4" width="3.7109375" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" customWidth="1"/>
+    <col min="6" max="6" width="41.140625" customWidth="1"/>
+    <col min="7" max="23" width="5.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -508,58 +514,58 @@
         <v>1</v>
       </c>
       <c r="G1" s="5">
-        <v>44700.0</v>
+        <v>44700</v>
       </c>
       <c r="H1" s="5">
-        <v>44707.0</v>
+        <v>44707</v>
       </c>
       <c r="I1" s="5">
-        <v>44714.0</v>
+        <v>44714</v>
       </c>
       <c r="J1" s="5">
-        <v>44721.0</v>
+        <v>44721</v>
       </c>
       <c r="K1" s="5">
-        <v>44728.0</v>
+        <v>44728</v>
       </c>
       <c r="L1" s="5">
-        <v>44735.0</v>
+        <v>44735</v>
       </c>
       <c r="M1" s="5">
-        <v>44742.0</v>
+        <v>44742</v>
       </c>
       <c r="N1" s="5">
-        <v>44749.0</v>
+        <v>44749</v>
       </c>
       <c r="O1" s="5">
-        <v>44756.0</v>
+        <v>44756</v>
       </c>
       <c r="P1" s="5">
-        <v>44763.0</v>
+        <v>44763</v>
       </c>
       <c r="Q1" s="5">
-        <v>44770.0</v>
+        <v>44770</v>
       </c>
       <c r="R1" s="5">
-        <v>44777.0</v>
+        <v>44777</v>
       </c>
       <c r="S1" s="5">
-        <v>44784.0</v>
+        <v>44784</v>
       </c>
       <c r="T1" s="5">
-        <v>44791.0</v>
+        <v>44791</v>
       </c>
       <c r="U1" s="5">
-        <v>44798.0</v>
+        <v>44798</v>
       </c>
       <c r="V1" s="5">
-        <v>44805.0</v>
+        <v>44805</v>
       </c>
       <c r="W1" s="5">
-        <v>44812.0</v>
-      </c>
-    </row>
-    <row r="2">
+        <v>44812</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="6"/>
@@ -588,7 +594,7 @@
       <c r="V2" s="10"/>
       <c r="W2" s="10"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="6"/>
@@ -617,7 +623,7 @@
       <c r="V3" s="10"/>
       <c r="W3" s="10"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" s="12"/>
       <c r="B4" s="3"/>
       <c r="C4" s="6"/>
@@ -646,7 +652,7 @@
       <c r="V4" s="10"/>
       <c r="W4" s="10"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" s="13"/>
       <c r="B5" s="15" t="s">
         <v>6</v>
@@ -677,7 +683,7 @@
       <c r="V5" s="10"/>
       <c r="W5" s="10"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" s="16"/>
       <c r="B6" s="15" t="s">
         <v>8</v>
@@ -686,14 +692,14 @@
       <c r="D6" s="6"/>
       <c r="E6" s="13"/>
       <c r="F6" s="14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G6" s="10"/>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="11"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
       <c r="K6" s="10"/>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
@@ -708,19 +714,23 @@
       <c r="V6" s="10"/>
       <c r="W6" s="10"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="13"/>
-      <c r="F7" s="14"/>
+      <c r="F7" s="14" t="s">
+        <v>11</v>
+      </c>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
+      <c r="J7" s="10" t="s">
+        <v>3</v>
+      </c>
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
@@ -735,7 +745,7 @@
       <c r="V7" s="10"/>
       <c r="W7" s="10"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -760,7 +770,7 @@
       <c r="V8" s="10"/>
       <c r="W8" s="10"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C10" s="17"/>
     </row>
   </sheetData>
@@ -769,9 +779,9 @@
       <formula>LEN(TRIM(C1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
atualizando cronograma e readme
</commit_message>
<xml_diff>
--- a/docs/Cronograma_Grupo4.xlsx
+++ b/docs/Cronograma_Grupo4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Facul\2022.1\Projeto e Contrucao de sistemas\Projeto\G1-P4-Airflow\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59AD576-9010-4745-B994-EDE0F0813340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21613F1-A89D-4433-A437-71D846BFD293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="690" yWindow="2295" windowWidth="21600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,7 +93,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -128,6 +128,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FF0000FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -174,16 +186,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -191,6 +199,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,7 +500,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="6" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H6" sqref="H6"/>
+      <selection pane="topRight" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -574,25 +586,25 @@
       <c r="F2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10"/>
-      <c r="W2" s="10"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
@@ -603,175 +615,175 @@
       <c r="F3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
-      <c r="V3" s="10"/>
-      <c r="W3" s="10"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="9"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A4" s="12"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="3"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="14" t="s">
+      <c r="E4" s="11"/>
+      <c r="F4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="11" t="s">
+      <c r="G4" s="9"/>
+      <c r="H4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
-      <c r="W4" s="10"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A5" s="13"/>
-      <c r="B5" s="15" t="s">
+      <c r="A5" s="11"/>
+      <c r="B5" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="14" t="s">
+      <c r="E5" s="11"/>
+      <c r="F5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="11" t="s">
+      <c r="G5" s="9"/>
+      <c r="H5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
-      <c r="U5" s="10"/>
-      <c r="V5" s="10"/>
-      <c r="W5" s="10"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="9"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A6" s="16"/>
-      <c r="B6" s="15" t="s">
+      <c r="A6" s="14"/>
+      <c r="B6" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="14" t="s">
+      <c r="E6" s="11"/>
+      <c r="F6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10" t="s">
+      <c r="G6" s="9"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
-      <c r="V6" s="10"/>
-      <c r="W6" s="10"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="14" t="s">
+      <c r="E7" s="11"/>
+      <c r="F7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10" t="s">
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="10"/>
-      <c r="S7" s="10"/>
-      <c r="T7" s="10"/>
-      <c r="U7" s="10"/>
-      <c r="V7" s="10"/>
-      <c r="W7" s="10"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="10"/>
-      <c r="U8" s="10"/>
-      <c r="V8" s="10"/>
-      <c r="W8" s="10"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="C10" s="17"/>
+      <c r="C10" s="15"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:D1">

</xml_diff>

<commit_message>
atualizando cronograma; atualizando readme
</commit_message>
<xml_diff>
--- a/docs/Cronograma_Grupo4.xlsx
+++ b/docs/Cronograma_Grupo4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Facul\2022.1\Projeto e Contrucao de sistemas\Projeto\G1-P4-Airflow\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21613F1-A89D-4433-A437-71D846BFD293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC0FBF60-585E-4A00-9662-C10AAA633FD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="2295" windowWidth="21600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Página1" sheetId="1" r:id="rId1"/>
@@ -500,7 +500,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="6" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E14" sqref="E14"/>
+      <selection pane="topRight" activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -709,11 +709,11 @@
       <c r="G6" s="9"/>
       <c r="H6" s="10"/>
       <c r="I6" s="9"/>
-      <c r="J6" s="9" t="s">
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
       <c r="O6" s="9"/>
@@ -740,12 +740,12 @@
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
-      <c r="J7" s="9" t="s">
-        <v>3</v>
-      </c>
+      <c r="J7" s="9"/>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
+      <c r="M7" s="9" t="s">
+        <v>3</v>
+      </c>
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
       <c r="P7" s="9"/>

</xml_diff>